<commit_message>
translater traverses folder, writes generated tokens back to files
</commit_message>
<xml_diff>
--- a/genai/text.xlsx
+++ b/genai/text.xlsx
@@ -2,41 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Source\Repos\learning\genai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECA0125-C20C-4FE6-9AEE-1C5C60754868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6EDE99-114C-431D-9E1A-480D14CE9C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{54D5BA9A-B74C-4D13-ADA9-54C58B73744C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Translated_Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Translated_Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+  <si>
+    <t>hun</t>
+  </si>
   <si>
     <t>alma</t>
   </si>
@@ -50,23 +40,55 @@
     <t>panzerkraftwagen</t>
   </si>
   <si>
-    <t>hun</t>
-  </si>
-  <si>
-    <t>eng</t>
+    <t>körte</t>
+  </si>
+  <si>
+    <t>szék</t>
+  </si>
+  <si>
+    <t>Ez egy egész mondat.</t>
+  </si>
+  <si>
+    <t>translated_hun</t>
+  </si>
+  <si>
+    <t>['Apples']</t>
+  </si>
+  <si>
+    <t>["I don't think that's going to be difficult."]</t>
+  </si>
+  <si>
+    <t>["We'll see"]</t>
+  </si>
+  <si>
+    <t>['Other vehicles']</t>
+  </si>
+  <si>
+    <t>['the roasting']</t>
+  </si>
+  <si>
+    <t>['Other, of a kind used for the manufacture of goods']</t>
+  </si>
+  <si>
+    <t>["That's a whole sentence."]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +107,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,47 +464,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C677E1E-AC05-43B9-9EF0-E50B3BC78D51}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="33.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying to copy formatting an overwriting content on excel file
</commit_message>
<xml_diff>
--- a/genai/text.xlsx
+++ b/genai/text.xlsx
@@ -1,75 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Source\Repos\learning\genai\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA76D930-0C1B-405B-B03D-2B0F93523FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Translated_Sheet1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Translated_Sheet2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>hun</t>
-  </si>
-  <si>
-    <t>alma</t>
-  </si>
-  <si>
-    <t>nem gondolom, hogy ez nehezére esne</t>
-  </si>
-  <si>
-    <t>majd meglátjuk</t>
-  </si>
-  <si>
-    <t>panzerkraftwagen</t>
-  </si>
-  <si>
-    <t>körte</t>
-  </si>
-  <si>
-    <t>szék</t>
-  </si>
-  <si>
-    <t>Ez egy egész mondat.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,7 +52,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -107,30 +78,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -450,83 +489,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col width="32" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>magyar oszlop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>alma</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>nem gondolom, hogy ez nehezére esne</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" thickBot="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>majd meglátjuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" thickTop="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>panzerkraftwagen</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col width="18" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>magyar oszlop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>körte</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>szék</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ez egy egész mondat.</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>magyar oszlop</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>translated_magyar oszlop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>alma</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['Apples']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>nem gondolom, hogy ez nehezére esne</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>["I don't think that's going to be difficult."]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>majd meglátjuk</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>["We'll see"]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>panzerkraftwagen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['Other vehicles']</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>magyar oszlop</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>translated_magyar oszlop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>körte</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['the roasting']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>szék</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['Other, of a kind used for the manufacture of goods']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ez egy egész mondat.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>["That's a whole sentence."]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cell formatting finally works
</commit_message>
<xml_diff>
--- a/genai/text.xlsx
+++ b/genai/text.xlsx
@@ -602,76 +602,55 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="32" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>magyar oszlop</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>translated_magyar oszlop</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hungarian column</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>alma</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>['Apples']</t>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Apples</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>nem gondolom, hogy ez nehezére esne</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>["I don't think that's going to be difficult."]</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>majd meglátjuk</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>["We'll see"]</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>panzerkraftwagen</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>['Other vehicles']</t>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>I don't think that's going to be difficult.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" thickBot="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>We'll see</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" thickTop="1">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Other vehicles</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -681,63 +660,46 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="18" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>magyar oszlop</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>translated_magyar oszlop</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hungarian column</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>körte</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>['the roasting']</t>
+          <t>the roasting</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>szék</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>['Other, of a kind used for the manufacture of goods']</t>
+          <t>Other, of a kind used for the manufacture of goods</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ez egy egész mondat.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>["That's a whole sentence."]</t>
+          <t>That's a whole sentence.</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>